<commit_message>
validated ImportToTblDf and add Data_Ingestion_Overview.md
</commit_message>
<xml_diff>
--- a/tests/test_data/Example2.xlsx
+++ b/tests/test_data/Example2.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\j.d.landgrebe\Box Sync\Projects\Python_Col_Info\tests\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_Col_Info\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF93ACDA-1387-4531-A956-273629167E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52896DC2-022F-4B2F-8159-CC0AC09708CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19087" yWindow="2445" windowWidth="15375" windowHeight="11872" xr2:uid="{D791E7BB-7986-4084-9B03-31A22112046A}"/>
+    <workbookView xWindow="2760" yWindow="3135" windowWidth="28800" windowHeight="11587" xr2:uid="{D791E7BB-7986-4084-9B03-31A22112046A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data_dummy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -443,9 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016B0039-CBCC-4EA1-95CA-2A3C901C2C96}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -555,4 +554,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89192DC5-37B6-4716-9118-B07057516793}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>